<commit_message>
Central_America.xlsx: removed Cayambe because it doesn't work
</commit_message>
<xml_diff>
--- a/docs/Central_America.xlsx
+++ b/docs/Central_America.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/gxd593_miami_edu/Documents/scratch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giacomo/Library/CloudStorage/OneDrive-UniversityofMiami/stampede2/code/minsar/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{28CF9CC8-99FB-424A-A616-75753B857ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C90AFA6-8608-9F42-BF02-D972ACFB5CF1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FF58C1-260B-A84E-9ED5-356F6F08FAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20160" xr2:uid="{526A8971-ACCA-E146-9E73-F0ED309CE934}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20140" xr2:uid="{526A8971-ACCA-E146-9E73-F0ED309CE934}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -96,12 +96,6 @@
   </si>
   <si>
     <t>POLYGON((-77.6792 -0.1123,-77.6177 -0.1123,-77.6177 -0.0629,-77.6792 -0.0629,-77.6792 -0.1123))</t>
-  </si>
-  <si>
-    <t>Cayambe</t>
-  </si>
-  <si>
-    <t>POLYGON((-78.1073 -0.0718,-77.8851 -0.0718,-77.8851 0.1217,-78.1073 0.1217,-78.1073 -0.0718))</t>
   </si>
   <si>
     <t>POLYGON((-78.6425 -0.2151,-78.5145 -0.2151,-78.5145 -0.1217,-78.6425 -0.1217,-78.6425 -0.2151))</t>
@@ -195,10 +189,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -518,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867F7809-BA29-C745-8BA8-4CEEF61BE96C}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,7 +580,7 @@
         <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -619,7 +609,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -648,7 +638,7 @@
         <v>16</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -677,7 +667,7 @@
         <v>16</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -706,7 +696,7 @@
         <v>19</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -735,12 +725,12 @@
         <v>19</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -752,24 +742,24 @@
         <v>8</v>
       </c>
       <c r="E8" s="4">
-        <v>142</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>10</v>
+        <v>40</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -783,22 +773,22 @@
       <c r="E9" s="4">
         <v>120</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>18</v>
+      <c r="F9" s="4">
+        <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -810,24 +800,24 @@
         <v>8</v>
       </c>
       <c r="E10" s="4">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="F10" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
@@ -848,79 +838,43 @@
         <v>8</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3">
-        <v>20160701</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="4">
-        <v>142</v>
-      </c>
-      <c r="F12" s="4">
-        <v>3</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="3">
-        <v>20160701</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="4">
-        <v>120</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -931,7 +885,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -1110,28 +1064,6 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>